<commit_message>
jjerc frogs caught master list
</commit_message>
<xml_diff>
--- a/data_in/JJERC_Frogs_2013.xlsx
+++ b/data_in/JJERC_Frogs_2013.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="4635" windowHeight="9720"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="4635" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="export_jjerc" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="71">
   <si>
     <t>Trifluralin</t>
   </si>
@@ -219,6 +219,21 @@
   </si>
   <si>
     <t>ug/g</t>
+  </si>
+  <si>
+    <t>sample_id</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>ag</t>
   </si>
 </sst>
 </file>
@@ -580,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X75" sqref="S19:X75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4545,14 +4560,1674 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2">
+        <v>3.8357000000000001</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>7.5732605394209116E-3</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1.2835407312178727E-2</v>
+      </c>
+      <c r="H2" s="4">
+        <v>2.3755774382234564E-2</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3">
+        <v>4.9238</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6.6277201038878316E-3</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1.3286247127707974E-2</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4">
+        <v>4.8345000000000002</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>6.0053535128666621E-3</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5">
+        <v>5.9812000000000003</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>6.2782812472777809E-3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6">
+        <v>4.8632999999999997</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.631453954017946E-2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>6.8595373845801201E-3</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1.3491953507417135E-2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>2.2267185558557674E-2</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2.6020553457669661E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7">
+        <v>5.609</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.6067480776713255E-2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>6.2976945170894498E-3</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1.3121682023940645E-2</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8">
+        <v>5.0804999999999998</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>6.0955681196385378E-3</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9">
+        <v>6.2168000000000001</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1.7915347879162592E-2</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.0806140941587758E-2</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1.7472943361399713E-2</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2.5021346853521368E-2</v>
+      </c>
+      <c r="I9" s="4">
+        <v>3.2649232540441164E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5.3727999999999998</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2.8924220867165184E-2</v>
+      </c>
+      <c r="E10" s="4">
+        <v>6.8903702248692428E-3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>3.6156796705094613E-2</v>
+      </c>
+      <c r="H10" s="4">
+        <v>5.2107861392996419E-2</v>
+      </c>
+      <c r="I10" s="4">
+        <v>6.1165115404651541E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11">
+        <v>4.87</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>6.0122052551531344E-3</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1.2520562269901649E-2</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12">
+        <v>6.8170000000000002</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>6.2634358056570917E-3</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13">
+        <v>4.6210000000000004</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>6.5694802944528232E-3</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14">
+        <v>3.6217000000000001</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1.6024755525789573E-2</v>
+      </c>
+      <c r="E14" s="4">
+        <v>5.9779465437207755E-3</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1.2740553814868393E-2</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2.1824779135930197E-2</v>
+      </c>
+      <c r="I14" s="4">
+        <v>2.5130582122710108E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15">
+        <v>6.3460000000000001</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>6.7327801522803965E-3</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16">
+        <v>5.4550999999999998</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1.8634556269711278E-2</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.1040242136375538E-2</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1.751979870344458E-2</v>
+      </c>
+      <c r="H16" s="4">
+        <v>2.5670451358851848E-2</v>
+      </c>
+      <c r="I16" s="4">
+        <v>3.0140900783639745E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17">
+        <v>8.5421999999999993</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1.6156491716137599E-2</v>
+      </c>
+      <c r="E17" s="4">
+        <v>7.1495944747074179E-3</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18">
+        <v>5.4204999999999997</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>7.1507364317551633E-3</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1.2894262193039959E-2</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19">
+        <v>6.5655000000000001</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>6.2622938486093464E-3</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20">
+        <v>6.0563000000000002</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1.69540297333797E-2</v>
+      </c>
+      <c r="E20" s="4">
+        <v>7.9364028806039062E-3</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1.4171927373677975E-2</v>
+      </c>
+      <c r="H20" s="4">
+        <v>2.3177382378881426E-2</v>
+      </c>
+      <c r="I20" s="4">
+        <v>2.6780243817739705E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="2">
+        <v>5.4325999999999999</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="2">
+        <v>4.7656999999999998</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1.6177854341599438E-2</v>
+      </c>
+      <c r="E22" s="4">
+        <v>6.7236444958984343E-3</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1.2975973338313322E-2</v>
+      </c>
+      <c r="H22" s="4">
+        <v>2.204960862939662E-2</v>
+      </c>
+      <c r="I22" s="4">
+        <v>2.6443966626060595E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2.758</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>6.4575685037737878E-3</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4">
+        <v>2.5050213988849688E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="2">
+        <v>7.7217000000000002</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1.6129788434310295E-2</v>
+      </c>
+      <c r="E24" s="4">
+        <v>7.0799350947949573E-3</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1.2886833907106017E-2</v>
+      </c>
+      <c r="H24" s="4">
+        <v>2.1958951575579512E-2</v>
+      </c>
+      <c r="I24" s="4">
+        <v>2.6177482813786585E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3.2128000000000001</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1.6703018884203058E-2</v>
+      </c>
+      <c r="E25" s="4">
+        <v>7.4990333313174687E-3</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>1.4186783945545858E-2</v>
+      </c>
+      <c r="H25" s="4">
+        <v>2.3389519884813453E-2</v>
+      </c>
+      <c r="I25" s="4">
+        <v>2.874503319553778E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="2">
+        <v>6.9470000000000001</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1.6314931188312929E-2</v>
+      </c>
+      <c r="E26" s="4">
+        <v>7.0102757148824959E-3</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>1.2992544130012116E-2</v>
+      </c>
+      <c r="H26" s="4">
+        <v>2.2399544857130652E-2</v>
+      </c>
+      <c r="I26" s="4">
+        <v>2.5526077939338997E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="2">
+        <v>4.2332999999999998</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1.6006953337904705E-2</v>
+      </c>
+      <c r="E27" s="4">
+        <v>6.1047037760205E-3</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0</v>
+      </c>
+      <c r="G27" s="4">
+        <v>1.2767409925552644E-2</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4">
+        <v>2.5320927702905827E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3.0754999999999999</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1.6311370750735951E-2</v>
+      </c>
+      <c r="E28" s="4">
+        <v>6.7362060234236317E-3</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4">
+        <v>1.3318245897884955E-2</v>
+      </c>
+      <c r="H28" s="4">
+        <v>2.2038729782938568E-2</v>
+      </c>
+      <c r="I28" s="4">
+        <v>2.6866956804273315E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="2">
+        <v>7.4720000000000004</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1.7424007493540228E-2</v>
+      </c>
+      <c r="E29" s="4">
+        <v>7.8838728564076255E-3</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="4">
+        <v>1.4477058503579898E-2</v>
+      </c>
+      <c r="H29" s="4">
+        <v>2.3561768287065955E-2</v>
+      </c>
+      <c r="I29" s="4">
+        <v>2.7298406786050288E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="2">
+        <v>6.165</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1.6468030004122794E-2</v>
+      </c>
+      <c r="E30" s="4">
+        <v>7.9581000645110658E-3</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4">
+        <v>1.3509667112336535E-2</v>
+      </c>
+      <c r="H30" s="4">
+        <v>2.2551848707543388E-2</v>
+      </c>
+      <c r="I30" s="4">
+        <v>2.9032666516722431E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="2">
+        <v>5.9501999999999997</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1.6174293904022467E-2</v>
+      </c>
+      <c r="E31" s="4">
+        <v>7.1553042599461448E-3</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>1.2875405774899954E-2</v>
+      </c>
+      <c r="H31" s="4">
+        <v>2.1877360227144118E-2</v>
+      </c>
+      <c r="I31" s="4">
+        <v>2.6947324938133729E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="2">
+        <v>5.9518000000000004</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1.9188204312930678E-2</v>
+      </c>
+      <c r="E32" s="4">
+        <v>1.2535063911874089E-2</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>1.8611756735734047E-2</v>
+      </c>
+      <c r="H32" s="4">
+        <v>2.6955968381978418E-2</v>
+      </c>
+      <c r="I32" s="4">
+        <v>3.1208950983626863E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="2">
+        <v>5.8708</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0</v>
+      </c>
+      <c r="E33" s="4">
+        <v>6.4061804366252507E-3</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4">
+        <v>1.269255565960292E-2</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0</v>
+      </c>
+      <c r="I33" s="4">
+        <v>2.5215180158352651E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2.5663</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0</v>
+      </c>
+      <c r="G34" s="4">
+        <v>0</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0</v>
+      </c>
+      <c r="I34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="2">
+        <v>4.0613999999999999</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+      <c r="E35" s="4">
+        <v>6.4678461172034954E-3</v>
+      </c>
+      <c r="F35" s="4">
+        <v>0</v>
+      </c>
+      <c r="G35" s="4">
+        <v>1.2874834368289649E-2</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0</v>
+      </c>
+      <c r="I35" s="4">
+        <v>2.5373801475182419E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="2">
+        <v>5.3468</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1.6124447777944837E-2</v>
+      </c>
+      <c r="E36" s="4">
+        <v>6.4575685037737878E-3</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0</v>
+      </c>
+      <c r="G36" s="4">
+        <v>1.2970259272210289E-2</v>
+      </c>
+      <c r="H36" s="4">
+        <v>2.1895491637907539E-2</v>
+      </c>
+      <c r="I36" s="4">
+        <v>2.5674124501713445E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="2">
+        <v>5.7293000000000003</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0</v>
+      </c>
+      <c r="G37" s="4">
+        <v>0</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0</v>
+      </c>
+      <c r="I37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="2">
+        <v>5.1879999999999997</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1.7240644958326085E-2</v>
+      </c>
+      <c r="E38" s="4">
+        <v>9.0829277565401528E-3</v>
+      </c>
+      <c r="F38" s="4">
+        <v>0</v>
+      </c>
+      <c r="G38" s="4">
+        <v>1.5517018534331769E-2</v>
+      </c>
+      <c r="H38" s="4">
+        <v>2.4218125356701804E-2</v>
+      </c>
+      <c r="I38" s="4">
+        <v>3.0189544654134211E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="2">
+        <v>6.6851000000000003</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0</v>
+      </c>
+      <c r="E39" s="4">
+        <v>0</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0</v>
+      </c>
+      <c r="G39" s="4">
+        <v>0</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0</v>
+      </c>
+      <c r="I39" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="2">
+        <v>7.1657000000000002</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1.6075117915315868E-2</v>
+      </c>
+      <c r="E40" s="4">
+        <v>6.4856263884368881E-3</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0</v>
+      </c>
+      <c r="G40" s="4">
+        <v>1.2951974260680586E-2</v>
+      </c>
+      <c r="H40" s="4">
+        <v>2.2036916641862223E-2</v>
+      </c>
+      <c r="I40" s="4">
+        <v>2.5397065934984118E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="2">
+        <v>4.7927999999999997</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0</v>
+      </c>
+      <c r="E41" s="4">
+        <v>0</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0</v>
+      </c>
+      <c r="G41" s="4">
+        <v>0</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0</v>
+      </c>
+      <c r="I41" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="2">
+        <v>5.7119999999999997</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0</v>
+      </c>
+      <c r="E42" s="4">
+        <v>0</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0</v>
+      </c>
+      <c r="G42" s="4">
+        <v>0</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0</v>
+      </c>
+      <c r="I42" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="2">
+        <v>4.6231999999999998</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1.5999832462750756E-2</v>
+      </c>
+      <c r="E43" s="4">
+        <v>6.4746978594899668E-3</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0</v>
+      </c>
+      <c r="G43" s="4">
+        <v>1.2706840824860502E-2</v>
+      </c>
+      <c r="H43" s="4">
+        <v>2.1968017280961226E-2</v>
+      </c>
+      <c r="I43" s="4">
+        <v>2.6465116134971232E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="2">
+        <v>13.578799999999999</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1.8554446424229362E-2</v>
+      </c>
+      <c r="E44" s="4">
+        <v>1.2273555747940425E-2</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0</v>
+      </c>
+      <c r="G44" s="4">
+        <v>2.1540215613538079E-2</v>
+      </c>
+      <c r="H44" s="4">
+        <v>2.7552491796094977E-2</v>
+      </c>
+      <c r="I44" s="4">
+        <v>3.2361599219256514E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="2">
+        <v>16.745000000000001</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
+      </c>
+      <c r="E45" s="4">
+        <v>6.64028163141303E-3</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0</v>
+      </c>
+      <c r="G45" s="4">
+        <v>1.3721087558148728E-2</v>
+      </c>
+      <c r="H45" s="4">
+        <v>0</v>
+      </c>
+      <c r="I45" s="4">
+        <v>2.5437250001914324E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="2">
+        <v>4.8734000000000002</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0</v>
+      </c>
+      <c r="E46" s="4">
+        <v>6.1138394324024622E-3</v>
+      </c>
+      <c r="F46" s="4">
+        <v>0</v>
+      </c>
+      <c r="G46" s="4">
+        <v>0</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="2">
+        <v>6.6909999999999998</v>
+      </c>
+      <c r="D47" s="4">
+        <v>1.6031876400943518E-2</v>
+      </c>
+      <c r="E47" s="4">
+        <v>1.1379403379555883E-2</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0</v>
+      </c>
+      <c r="G47" s="4">
+        <v>0</v>
+      </c>
+      <c r="H47" s="4">
+        <v>0</v>
+      </c>
+      <c r="I47" s="4">
+        <v>2.5492238725081981E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="2">
+        <v>11.2064</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0</v>
+      </c>
+      <c r="E48" s="4">
+        <v>7.338017387585387E-3</v>
+      </c>
+      <c r="F48" s="4">
+        <v>0</v>
+      </c>
+      <c r="G48" s="4">
+        <v>0</v>
+      </c>
+      <c r="H48" s="4">
+        <v>0</v>
+      </c>
+      <c r="I48" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="2">
+        <v>6.3754999999999997</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0</v>
+      </c>
+      <c r="E49" s="4">
+        <v>8.0540244565216693E-3</v>
+      </c>
+      <c r="F49" s="4">
+        <v>0</v>
+      </c>
+      <c r="G49" s="4">
+        <v>0</v>
+      </c>
+      <c r="H49" s="4">
+        <v>0</v>
+      </c>
+      <c r="I49" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="2">
+        <v>22.694500000000001</v>
+      </c>
+      <c r="D50" s="4">
+        <v>1.6033656619732006E-2</v>
+      </c>
+      <c r="E50" s="4">
+        <v>8.5896023119141976E-3</v>
+      </c>
+      <c r="F50" s="4">
+        <v>0</v>
+      </c>
+      <c r="G50" s="4">
+        <v>1.5116462500509209E-2</v>
+      </c>
+      <c r="H50" s="4">
+        <v>0</v>
+      </c>
+      <c r="I50" s="4">
+        <v>2.667238132229546E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="2">
+        <v>22.096800000000002</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0</v>
+      </c>
+      <c r="E51" s="4">
+        <v>7.443077435977951E-3</v>
+      </c>
+      <c r="F51" s="4">
+        <v>0</v>
+      </c>
+      <c r="G51" s="4">
+        <v>1.2626272492807747E-2</v>
+      </c>
+      <c r="H51" s="4">
+        <v>2.7148161336070682E-2</v>
+      </c>
+      <c r="I51" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="2">
+        <v>13.7539</v>
+      </c>
+      <c r="D52" s="4">
+        <v>0</v>
+      </c>
+      <c r="E52" s="4">
+        <v>9.2165367311263496E-3</v>
+      </c>
+      <c r="F52" s="4">
+        <v>0</v>
+      </c>
+      <c r="G52" s="4">
+        <v>1.2976544744923626E-2</v>
+      </c>
+      <c r="H52" s="4">
+        <v>2.639389464831236E-2</v>
+      </c>
+      <c r="I52" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="2">
+        <v>35.850099999999998</v>
+      </c>
+      <c r="D53" s="4">
+        <v>0</v>
+      </c>
+      <c r="E53" s="4">
+        <v>1.0248865902288068E-2</v>
+      </c>
+      <c r="F53" s="4">
+        <v>0</v>
+      </c>
+      <c r="G53" s="4">
+        <v>1.2803979948612052E-2</v>
+      </c>
+      <c r="H53" s="4">
+        <v>5.9539926664922804E-2</v>
+      </c>
+      <c r="I53" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="2">
+        <v>17.1082</v>
+      </c>
+      <c r="D54" s="4">
+        <v>0</v>
+      </c>
+      <c r="E54" s="4">
+        <v>9.6881649918451433E-3</v>
+      </c>
+      <c r="F54" s="4">
+        <v>0</v>
+      </c>
+      <c r="G54" s="4">
+        <v>1.2814265267597507E-2</v>
+      </c>
+      <c r="H54" s="4">
+        <v>2.7033933448261129E-2</v>
+      </c>
+      <c r="I54" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="2">
+        <v>17.1082</v>
+      </c>
+      <c r="D55" s="4">
+        <v>0</v>
+      </c>
+      <c r="E55" s="4">
+        <v>1.0502380366887517E-2</v>
+      </c>
+      <c r="F55" s="4">
+        <v>0</v>
+      </c>
+      <c r="G55" s="4">
+        <v>1.2715983330625354E-2</v>
+      </c>
+      <c r="H55" s="4">
+        <v>3.5941895556330004E-2</v>
+      </c>
+      <c r="I55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="2">
+        <v>30.857199999999999</v>
+      </c>
+      <c r="D56" s="4">
+        <v>0</v>
+      </c>
+      <c r="E56" s="4">
+        <v>6.5797579078825308E-3</v>
+      </c>
+      <c r="F56" s="4">
+        <v>0</v>
+      </c>
+      <c r="G56" s="4">
+        <v>0</v>
+      </c>
+      <c r="H56" s="4">
+        <v>6.8431570503304603E-2</v>
+      </c>
+      <c r="I56" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="2">
+        <v>20.395299999999999</v>
+      </c>
+      <c r="D57" s="4">
+        <v>1.5944645680307665E-2</v>
+      </c>
+      <c r="E57" s="4">
+        <v>6.9954302732618068E-3</v>
+      </c>
+      <c r="F57" s="4">
+        <v>0</v>
+      </c>
+      <c r="G57" s="4">
+        <v>1.2843407004722973E-2</v>
+      </c>
+      <c r="H57" s="4">
+        <v>7.4237248229752098E-2</v>
+      </c>
+      <c r="I57" s="4">
+        <v>2.6691415880315032E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>